<commit_message>
Created a openapi specs folder
</commit_message>
<xml_diff>
--- a/00-Design Docs Folder/Design.xlsx
+++ b/00-Design Docs Folder/Design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/go/src/starships/00-Design Docs Folder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/go/src/starship/00-Design Docs Folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37640C01-1658-384A-A0FE-89134E0E9A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AA7781-D580-BD45-A3FC-267278AEF875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{4F7DAF7F-279B-6447-B135-A3CF6EEEB132}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
   <si>
     <t>Project Name:</t>
   </si>
@@ -376,6 +376,9 @@
   </si>
   <si>
     <t>Data Requirements</t>
+  </si>
+  <si>
+    <t>/imperialship { id }</t>
   </si>
 </sst>
 </file>
@@ -464,35 +467,16 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -501,6 +485,25 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -817,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3735BF52-4F22-B545-8528-7EB44C375E7F}">
   <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A40" zoomScale="130" zoomScaleNormal="153" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="130" zoomScaleNormal="153" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -829,16 +832,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -846,15 +849,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -863,7 +866,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
@@ -872,7 +875,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
@@ -887,7 +890,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="E8" t="s">
         <v>19</v>
       </c>
@@ -897,7 +900,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
@@ -906,7 +909,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
@@ -915,7 +918,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
@@ -924,7 +927,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
@@ -935,59 +938,59 @@
       <c r="A13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17" s="4"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18" s="4"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:7" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19"/>
-      <c r="B19" s="4"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
+      <c r="B19" s="3"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20"/>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="13"/>
       <c r="D20" t="s">
         <v>36</v>
       </c>
@@ -997,416 +1000,416 @@
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="10" t="s">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="10" t="s">
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23"/>
-      <c r="B23" s="4"/>
-      <c r="D23" s="10" t="s">
+      <c r="B23" s="3"/>
+      <c r="D23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="E23" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24"/>
-      <c r="B24" s="4"/>
-      <c r="D24" s="8" t="s">
+      <c r="B24" s="3"/>
+      <c r="D24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25"/>
-      <c r="B25" s="4"/>
-      <c r="D25" s="7" t="s">
+      <c r="B25" s="3"/>
+      <c r="D25" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26"/>
-      <c r="B26" s="4"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="B26" s="3"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27"/>
-      <c r="B27" s="4"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="B27" s="3"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28"/>
-      <c r="B28" s="4"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+      <c r="B28" s="3"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29"/>
-      <c r="B29" s="4"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
+      <c r="B29" s="3"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30"/>
-      <c r="B30" s="4"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
+      <c r="B30" s="3"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31"/>
-      <c r="B31" s="4"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="B31" s="3"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32"/>
-      <c r="B32" s="4"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
+      <c r="B32" s="3"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33"/>
-      <c r="B33" s="4"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
+      <c r="B33" s="3"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34"/>
-      <c r="B34" s="4"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
+      <c r="B34" s="3"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35"/>
-      <c r="B35" s="4"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
+      <c r="B35" s="3"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36"/>
-      <c r="B36" s="4"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
+      <c r="B36" s="3"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37"/>
-      <c r="B37" s="4"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38"/>
-      <c r="B38" s="4"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="B38" s="3"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39"/>
-      <c r="B39" s="4"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
+      <c r="B39" s="3"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40"/>
-      <c r="B40" s="4"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
+      <c r="B40" s="3"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41"/>
-      <c r="B41" s="4"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
+      <c r="B41" s="3"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42"/>
-      <c r="B42" s="4"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
+      <c r="B42" s="3"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43"/>
-      <c r="B43" s="4"/>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
+      <c r="B43" s="3"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44"/>
-      <c r="B44" s="4"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
+      <c r="B44" s="3"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45"/>
-      <c r="B45" s="4"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
+      <c r="B45" s="3"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46"/>
-      <c r="B46" s="4"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
+      <c r="B46" s="3"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47"/>
-      <c r="B47" s="4"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
+      <c r="B47" s="3"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
     </row>
     <row r="48" spans="1:7" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48"/>
-      <c r="B48" s="4"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
+      <c r="B48" s="3"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49"/>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50"/>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4" t="s">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4" t="s">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53"/>
-      <c r="B53" s="4"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
+      <c r="B53" s="3"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54"/>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="8" t="s">
+      <c r="C54" s="15"/>
+      <c r="D54" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60"/>
-      <c r="B60" s="4"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
+      <c r="B60" s="3"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61"/>
-      <c r="B61" s="4"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
+      <c r="B61" s="3"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62"/>
-      <c r="B62" s="4"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
+      <c r="B62" s="3"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63"/>
-      <c r="B63" s="4"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
+      <c r="B63" s="3"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64"/>
-      <c r="B64" s="4"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
+      <c r="B64" s="3"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65"/>
-      <c r="B65" s="4"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
+      <c r="B65" s="3"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
     </row>
     <row r="66" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66"/>
-      <c r="B66" s="4"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="8"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="8"/>
+      <c r="B66" s="3"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
     </row>
     <row r="67" spans="1:7" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67"/>
-      <c r="B67" s="4"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="10"/>
+      <c r="B67" s="3"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68"/>
-      <c r="B68" s="11" t="s">
+      <c r="B68" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C68" s="11"/>
+      <c r="C68" s="13"/>
       <c r="D68" t="s">
         <v>36</v>
       </c>
@@ -1416,479 +1419,479 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
       <c r="D69" t="s">
         <v>40</v>
       </c>
-      <c r="E69" s="13" t="s">
+      <c r="E69" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70"/>
-      <c r="B70" s="4"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10" t="s">
+      <c r="B70" s="3"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71"/>
-      <c r="B71" s="4"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="14" t="s">
+      <c r="B71" s="3"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="F71" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G71" s="8"/>
+      <c r="G71" s="10"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72"/>
-      <c r="B72" s="4"/>
-      <c r="D72" s="10"/>
-      <c r="E72" s="14" t="s">
+      <c r="B72" s="3"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F72" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G72" s="8"/>
+      <c r="G72" s="10"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73"/>
-      <c r="B73" s="4"/>
-      <c r="D73" s="10"/>
-      <c r="E73" s="14" t="s">
+      <c r="B73" s="3"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F73" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G73" s="8"/>
+      <c r="G73" s="10"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74"/>
-      <c r="B74" s="4"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="14" t="s">
+      <c r="B74" s="3"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F74" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G74" s="8"/>
+      <c r="G74" s="10"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75"/>
-      <c r="B75" s="4"/>
-      <c r="D75" s="10"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
+      <c r="B75" s="3"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76"/>
-      <c r="B76" s="4"/>
-      <c r="D76" s="10"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="10"/>
-      <c r="G76" s="10"/>
+      <c r="B76" s="3"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77"/>
-      <c r="B77" s="4"/>
-      <c r="D77" s="10"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="10"/>
-      <c r="G77" s="10"/>
+      <c r="B77" s="3"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78"/>
-      <c r="B78" s="4"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="10"/>
-      <c r="G78" s="10"/>
+      <c r="B78" s="3"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79"/>
-      <c r="B79" s="4"/>
-      <c r="D79" s="10"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="10"/>
-      <c r="G79" s="10"/>
+      <c r="B79" s="3"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80"/>
-      <c r="B80" s="4"/>
-      <c r="D80" s="10"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="10"/>
-      <c r="G80" s="10"/>
+      <c r="B80" s="3"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="5"/>
+      <c r="G80" s="5"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81"/>
-      <c r="B81" s="4"/>
-      <c r="D81" s="10"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="10"/>
-      <c r="G81" s="10"/>
+      <c r="B81" s="3"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="5"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82"/>
-      <c r="B82" s="4"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="10"/>
-      <c r="G82" s="10"/>
+      <c r="B82" s="3"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="5"/>
+      <c r="G82" s="5"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83"/>
-      <c r="B83" s="4"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="10"/>
-      <c r="G83" s="10"/>
+      <c r="B83" s="3"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="5"/>
+      <c r="G83" s="5"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84"/>
-      <c r="B84" s="4"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="10"/>
-      <c r="G84" s="10"/>
+      <c r="B84" s="3"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85"/>
-      <c r="B85" s="4"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="10"/>
-      <c r="G85" s="10"/>
+      <c r="B85" s="3"/>
+      <c r="D85" s="5"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86"/>
-      <c r="B86" s="4"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="10"/>
-      <c r="G86" s="10"/>
+      <c r="B86" s="3"/>
+      <c r="D86" s="5"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87"/>
-      <c r="B87" s="4"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="10"/>
-      <c r="G87" s="10"/>
+      <c r="B87" s="3"/>
+      <c r="D87" s="5"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88"/>
-      <c r="B88" s="4"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
+      <c r="B88" s="3"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89"/>
-      <c r="B89" s="4"/>
-      <c r="D89" s="10"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="10"/>
-      <c r="G89" s="10"/>
+      <c r="B89" s="3"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90"/>
-      <c r="B90" s="4"/>
-      <c r="D90" s="10"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="10"/>
-      <c r="G90" s="10"/>
+      <c r="B90" s="3"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91"/>
-      <c r="B91" s="4"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="10"/>
-      <c r="G91" s="10"/>
+      <c r="B91" s="3"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92"/>
-      <c r="B92" s="4"/>
-      <c r="D92" s="10"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="10"/>
-      <c r="G92" s="10"/>
+      <c r="B92" s="3"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93"/>
-      <c r="B93" s="4"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="10"/>
-      <c r="G93" s="10"/>
+      <c r="B93" s="3"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94"/>
-      <c r="B94" s="4"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="10"/>
-      <c r="G94" s="10"/>
+      <c r="B94" s="3"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95"/>
-      <c r="B95" s="4"/>
-      <c r="D95" s="10"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="10"/>
-      <c r="G95" s="10"/>
+      <c r="B95" s="3"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96"/>
-      <c r="B96" s="4"/>
-      <c r="D96" s="10"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="10"/>
-      <c r="G96" s="10"/>
+      <c r="B96" s="3"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97"/>
-      <c r="B97" s="4"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="14"/>
-      <c r="F97" s="10"/>
-      <c r="G97" s="10"/>
+      <c r="B97" s="3"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98"/>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="10"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99"/>
-      <c r="B99" s="6" t="s">
+      <c r="B99" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C99" s="6"/>
-      <c r="D99" s="8" t="s">
+      <c r="C99" s="15"/>
+      <c r="D99" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="8"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="8"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101"/>
-      <c r="B101" s="4"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="8"/>
+      <c r="B101" s="3"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102"/>
-      <c r="B102" s="4"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="8"/>
+      <c r="B102" s="3"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103"/>
-      <c r="B103" s="4"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="8"/>
+      <c r="B103" s="3"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104"/>
-      <c r="B104" s="4"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="8"/>
+      <c r="B104" s="3"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="G104" s="10"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105"/>
-      <c r="B105" s="4"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="8"/>
+      <c r="B105" s="3"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106"/>
-      <c r="B106" s="4"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="8"/>
+      <c r="B106" s="3"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107"/>
-      <c r="B107" s="4"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="8"/>
+      <c r="B107" s="3"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108"/>
-      <c r="B108" s="4"/>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8"/>
-      <c r="F108" s="8"/>
-      <c r="G108" s="8"/>
+      <c r="B108" s="3"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="10"/>
+      <c r="F108" s="10"/>
+      <c r="G108" s="10"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109"/>
-      <c r="B109" s="4"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="8"/>
+      <c r="B109" s="3"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="10"/>
+      <c r="F109" s="10"/>
+      <c r="G109" s="10"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110"/>
-      <c r="B110" s="4"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="8"/>
+      <c r="B110" s="3"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="10"/>
+      <c r="F110" s="10"/>
+      <c r="G110" s="10"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111"/>
-      <c r="B111" s="4"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="8"/>
+      <c r="B111" s="3"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10"/>
+      <c r="G111" s="10"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112"/>
-      <c r="B112" s="4"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
+      <c r="B112" s="3"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
+      <c r="F112" s="10"/>
+      <c r="G112" s="10"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113"/>
-      <c r="B113" s="4"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="8"/>
+      <c r="B113" s="3"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="10"/>
+      <c r="F113" s="10"/>
+      <c r="G113" s="10"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114"/>
-      <c r="B114" s="4"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="8"/>
+      <c r="B114" s="3"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="10"/>
+      <c r="F114" s="10"/>
+      <c r="G114" s="10"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115"/>
-      <c r="B115" s="4"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="8"/>
+      <c r="B115" s="3"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="10"/>
+      <c r="F115" s="10"/>
+      <c r="G115" s="10"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116"/>
-      <c r="B116" s="4"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="8"/>
+      <c r="B116" s="3"/>
+      <c r="D116" s="10"/>
+      <c r="E116" s="10"/>
+      <c r="F116" s="10"/>
+      <c r="G116" s="10"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117"/>
-      <c r="B117" s="4"/>
-      <c r="D117" s="8"/>
-      <c r="E117" s="8"/>
-      <c r="F117" s="8"/>
-      <c r="G117" s="8"/>
+      <c r="B117" s="3"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="10"/>
+      <c r="F117" s="10"/>
+      <c r="G117" s="10"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118"/>
-      <c r="B118" s="4"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="8"/>
+      <c r="B118" s="3"/>
+      <c r="D118" s="10"/>
+      <c r="E118" s="10"/>
+      <c r="F118" s="10"/>
+      <c r="G118" s="10"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119"/>
-      <c r="B119" s="4"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="8"/>
+      <c r="B119" s="3"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="10"/>
+      <c r="F119" s="10"/>
+      <c r="G119" s="10"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120"/>
-      <c r="B120" s="4"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="8"/>
+      <c r="B120" s="3"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="10"/>
+      <c r="F120" s="10"/>
+      <c r="G120" s="10"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121"/>
-      <c r="B121" s="4"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
-      <c r="F121" s="8"/>
-      <c r="G121" s="8"/>
+      <c r="B121" s="3"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="10"/>
+      <c r="F121" s="10"/>
+      <c r="G121" s="10"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122"/>
-      <c r="B122" s="4"/>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="8"/>
+      <c r="B122" s="3"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="10"/>
+      <c r="F122" s="10"/>
+      <c r="G122" s="10"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123"/>
-      <c r="B123" s="4"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="10"/>
-      <c r="F123" s="10"/>
-      <c r="G123" s="10"/>
+      <c r="B123" s="3"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="5"/>
+      <c r="G123" s="5"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124"/>
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C124" s="11"/>
+      <c r="C124" s="13"/>
       <c r="D124" t="s">
         <v>36</v>
       </c>
@@ -1898,167 +1901,167 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125"/>
-      <c r="B125" s="12"/>
-      <c r="C125" s="12"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="6"/>
       <c r="D125" t="s">
         <v>40</v>
       </c>
-      <c r="E125" s="13" t="s">
+      <c r="E125" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F125" s="13"/>
-      <c r="G125" s="13"/>
+      <c r="F125" s="12"/>
+      <c r="G125" s="12"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126"/>
-      <c r="C126" s="4"/>
+      <c r="C126" s="3"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127"/>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B128" s="6" t="s">
+      <c r="B128" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C128" s="6"/>
-      <c r="D128" s="8" t="s">
+      <c r="C128" s="15"/>
+      <c r="D128" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E128" s="8"/>
-      <c r="F128" s="8"/>
-      <c r="G128" s="8"/>
+      <c r="E128" s="10"/>
+      <c r="F128" s="10"/>
+      <c r="G128" s="10"/>
     </row>
     <row r="129" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="10"/>
+      <c r="F129" s="10"/>
+      <c r="G129" s="10"/>
     </row>
     <row r="130" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="8"/>
+      <c r="D130" s="10"/>
+      <c r="E130" s="10"/>
+      <c r="F130" s="10"/>
+      <c r="G130" s="10"/>
     </row>
     <row r="131" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
     </row>
     <row r="132" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D132" s="8"/>
-      <c r="E132" s="8"/>
-      <c r="F132" s="8"/>
-      <c r="G132" s="8"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="10"/>
+      <c r="F132" s="10"/>
+      <c r="G132" s="10"/>
     </row>
     <row r="133" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
-      <c r="F133" s="8"/>
-      <c r="G133" s="8"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+      <c r="F133" s="10"/>
+      <c r="G133" s="10"/>
     </row>
     <row r="134" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D134" s="8"/>
-      <c r="E134" s="8"/>
-      <c r="F134" s="8"/>
-      <c r="G134" s="8"/>
+      <c r="D134" s="10"/>
+      <c r="E134" s="10"/>
+      <c r="F134" s="10"/>
+      <c r="G134" s="10"/>
     </row>
     <row r="135" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D135" s="8"/>
-      <c r="E135" s="8"/>
-      <c r="F135" s="8"/>
-      <c r="G135" s="8"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="10"/>
+      <c r="F135" s="10"/>
+      <c r="G135" s="10"/>
     </row>
     <row r="136" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D136" s="8"/>
-      <c r="E136" s="8"/>
-      <c r="F136" s="8"/>
-      <c r="G136" s="8"/>
+      <c r="D136" s="10"/>
+      <c r="E136" s="10"/>
+      <c r="F136" s="10"/>
+      <c r="G136" s="10"/>
     </row>
     <row r="137" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
-      <c r="F137" s="8"/>
-      <c r="G137" s="8"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
     </row>
     <row r="138" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D138" s="8"/>
-      <c r="E138" s="8"/>
-      <c r="F138" s="8"/>
-      <c r="G138" s="8"/>
+      <c r="D138" s="10"/>
+      <c r="E138" s="10"/>
+      <c r="F138" s="10"/>
+      <c r="G138" s="10"/>
     </row>
     <row r="139" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D139" s="8"/>
-      <c r="E139" s="8"/>
-      <c r="F139" s="8"/>
-      <c r="G139" s="8"/>
+      <c r="D139" s="10"/>
+      <c r="E139" s="10"/>
+      <c r="F139" s="10"/>
+      <c r="G139" s="10"/>
     </row>
     <row r="140" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D140" s="8"/>
-      <c r="E140" s="8"/>
-      <c r="F140" s="8"/>
-      <c r="G140" s="8"/>
+      <c r="D140" s="10"/>
+      <c r="E140" s="10"/>
+      <c r="F140" s="10"/>
+      <c r="G140" s="10"/>
     </row>
     <row r="141" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D141" s="8"/>
-      <c r="E141" s="8"/>
-      <c r="F141" s="8"/>
-      <c r="G141" s="8"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
     </row>
     <row r="142" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D142" s="8"/>
-      <c r="E142" s="8"/>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8"/>
+      <c r="D142" s="10"/>
+      <c r="E142" s="10"/>
+      <c r="F142" s="10"/>
+      <c r="G142" s="10"/>
     </row>
     <row r="143" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D143" s="8"/>
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
     </row>
     <row r="144" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D144" s="8"/>
-      <c r="E144" s="8"/>
-      <c r="F144" s="8"/>
-      <c r="G144" s="8"/>
+      <c r="D144" s="10"/>
+      <c r="E144" s="10"/>
+      <c r="F144" s="10"/>
+      <c r="G144" s="10"/>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D145" s="8"/>
-      <c r="E145" s="8"/>
-      <c r="F145" s="8"/>
-      <c r="G145" s="8"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="10"/>
+      <c r="F145" s="10"/>
+      <c r="G145" s="10"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D146" s="8"/>
-      <c r="E146" s="8"/>
-      <c r="F146" s="8"/>
-      <c r="G146" s="8"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="10"/>
+      <c r="G146" s="10"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
-      <c r="F147" s="8"/>
-      <c r="G147" s="8"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148"/>
-      <c r="B148" s="4"/>
-      <c r="D148" s="10"/>
-      <c r="E148" s="10"/>
-      <c r="F148" s="10"/>
-      <c r="G148" s="10"/>
+      <c r="B148" s="3"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="5"/>
+      <c r="G148" s="5"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149"/>
-      <c r="B149" s="11" t="s">
+      <c r="B149" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C149" s="11"/>
+      <c r="C149" s="13"/>
       <c r="D149" t="s">
         <v>36</v>
       </c>
@@ -2070,11 +2073,11 @@
       <c r="D150" t="s">
         <v>40</v>
       </c>
-      <c r="E150" s="13" t="s">
+      <c r="E150" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F150" s="13"/>
-      <c r="G150" s="13"/>
+      <c r="F150" s="12"/>
+      <c r="G150" s="12"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D151" t="s">
@@ -2086,11 +2089,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="D49:G53"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="E125:G125"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D54:G66"/>
+    <mergeCell ref="D16:G18"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B124:C124"/>
     <mergeCell ref="E150:G150"/>
     <mergeCell ref="B149:C149"/>
@@ -2107,12 +2110,12 @@
     <mergeCell ref="B99:C99"/>
     <mergeCell ref="B128:C128"/>
     <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D49:G53"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="E125:G125"/>
     <mergeCell ref="F71:G71"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D54:G66"/>
-    <mergeCell ref="D16:G18"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="96" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2134,16 +2137,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -2151,7 +2154,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
@@ -2159,7 +2162,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
@@ -2173,7 +2176,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="E5" t="s">
         <v>19</v>
       </c>
@@ -2182,7 +2185,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
@@ -2190,7 +2193,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
@@ -2198,7 +2201,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
@@ -2206,7 +2209,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
@@ -2214,10 +2217,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>